<commit_message>
more flexible input fields
</commit_message>
<xml_diff>
--- a/example/jabil_jouse_template_for_print/jabil_jouse_template_for_print.xlsx
+++ b/example/jabil_jouse_template_for_print/jabil_jouse_template_for_print.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\头马会议经理文件包\tmma_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DFFF24-82AC-4F3B-A9CA-B3CA24EA6125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2669E6B1-D961-4238-9D3B-82FCA9E86C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="166">
   <si>
     <r>
       <rPr>
@@ -111,34 +111,6 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>日期</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t>118</t>
     </r>
     <r>
@@ -609,9 +581,6 @@
     <t>即兴主持人</t>
   </si>
   <si>
-    <t>备稿演讲项目简介</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="9"/>
@@ -681,9 +650,6 @@
       </rPr>
       <t>会员</t>
     </r>
-  </si>
-  <si>
-    <t>{project_info}</t>
   </si>
   <si>
     <t>即兴点评报告</t>
@@ -1854,12 +1820,6 @@
     <t>K24</t>
   </si>
   <si>
-    <t>images</t>
-  </si>
-  <si>
-    <t>A1,M1</t>
-  </si>
-  <si>
     <t>杨然（Alex Yang）</t>
   </si>
   <si>
@@ -1870,34 +1830,34 @@
   </si>
   <si>
     <t>林长宏（Leon Lin）</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>丘愉庄（Rainbow Qiu）</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>黎泳恩（Vivian Li)</t>
   </si>
   <si>
     <t>刘惠芳（Annie Liu）</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>N26</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>捷普聚思国际演讲俱乐部</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>（俱乐部号：5614337）</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>张合堂（Hunter Zhang）</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1986,7 +1946,7 @@
       </rPr>
       <t>）。</t>
     </r>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2001,11 +1961,62 @@
       </rPr>
       <t>时间：</t>
     </r>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>线上：</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>日期</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>备稿演讲项目简介</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>备稿演讲项目简介</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2056,11 +2067,6 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2235,6 +2241,13 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -2401,11 +2414,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2418,212 +2431,209 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="19" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="18" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="20" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="29" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="30" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="20" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2635,6 +2645,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2644,53 +2663,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3719,15 +3744,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>137520</xdr:colOff>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>16860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>596400</xdr:colOff>
+      <xdr:colOff>481740</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>171960</xdr:rowOff>
+      <xdr:rowOff>27180</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3746,8 +3771,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="137520" y="161640"/>
-          <a:ext cx="1361160" cy="1227960"/>
+          <a:off x="22860" y="16860"/>
+          <a:ext cx="1198020" cy="1077120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3762,15 +3787,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:colOff>777240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>188595</xdr:colOff>
+      <xdr:colOff>942975</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>81280</xdr:rowOff>
+      <xdr:rowOff>58420</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3793,7 +3818,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8328660" y="30480"/>
+          <a:off x="8549640" y="7620"/>
           <a:ext cx="950595" cy="919480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4109,8 +4134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4134,182 +4159,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="37.200000000000003">
-      <c r="A1" s="87"/>
-      <c r="B1" s="88"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="93" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="58" t="s">
-        <v>163</v>
-      </c>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="45"/>
+      <c r="A1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="98"/>
     </row>
     <row r="2" spans="1:1024" ht="31.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="91" t="s">
+      <c r="A2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="46"/>
-    </row>
-    <row r="3" spans="1:1024" s="4" customFormat="1" ht="15.6">
-      <c r="A3" s="89"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="38"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="99"/>
+    </row>
+    <row r="3" spans="1:1024" s="4" customFormat="1" ht="15.6" customHeight="1">
+      <c r="A3" s="95"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="39"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="47"/>
+      <c r="N3" s="99"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" s="4" customFormat="1" ht="15.6">
-      <c r="A4" s="89"/>
-      <c r="B4" s="90"/>
-      <c r="D4" s="94" t="s">
-        <v>166</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>2</v>
+    <row r="4" spans="1:1024" s="4" customFormat="1" ht="15.6" customHeight="1">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="D4" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>163</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="39" t="s">
+      <c r="J4" s="40"/>
+      <c r="K4" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="38"/>
+      <c r="N4" s="43"/>
+      <c r="AMJ4"/>
+    </row>
+    <row r="5" spans="1:1024" s="4" customFormat="1" ht="15.6">
+      <c r="A5" s="88" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="41" t="s">
         <v>3</v>
-      </c>
-      <c r="L4" s="39"/>
-      <c r="N4" s="46"/>
-      <c r="AMJ4"/>
-    </row>
-    <row r="5" spans="1:1024" s="4" customFormat="1" ht="15.6">
-      <c r="A5" s="95" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="42" t="s">
-        <v>4</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="N5" s="46"/>
+      <c r="N5" s="43"/>
       <c r="AMJ5"/>
     </row>
     <row r="6" spans="1:1024" s="4" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A6" s="48"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="38"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="L6" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" s="46"/>
+      <c r="L6" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="43"/>
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="54"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="50"/>
       <c r="AMJ7"/>
     </row>
     <row r="8" spans="1:1024" s="5" customFormat="1" ht="24" customHeight="1">
       <c r="A8" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="36" t="s">
+      <c r="J8" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="K8" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="84" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="84"/>
-      <c r="M8" s="84"/>
-      <c r="N8" s="84"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="92"/>
+      <c r="N8" s="92"/>
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="12" t="s">
+      <c r="J9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="K9" s="86" t="s">
         <v>14</v>
-      </c>
-      <c r="K9" s="86" t="s">
-        <v>15</v>
       </c>
       <c r="L9" s="86"/>
       <c r="M9" s="86"/>
@@ -4318,20 +4343,20 @@
     </row>
     <row r="10" spans="1:1024" s="4" customFormat="1" ht="22.8" customHeight="1">
       <c r="A10" s="85"/>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>17</v>
       </c>
       <c r="K10" s="86"/>
       <c r="L10" s="86"/>
@@ -4340,136 +4365,136 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="15" t="s">
+      <c r="H11" s="16" t="s">
         <v>20</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>21</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
-      <c r="K11" s="68" t="s">
+      <c r="K11" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="AMJ11"/>
+    </row>
+    <row r="12" spans="1:1024" s="6" customFormat="1" ht="24" customHeight="1">
+      <c r="A12" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="68"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
-      <c r="AMJ11"/>
-    </row>
-    <row r="12" spans="1:1024" s="6" customFormat="1" ht="24" customHeight="1">
-      <c r="A12" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="12" t="s">
+      <c r="J12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="K12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="21" t="s">
+      <c r="L12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="M12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="N12" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="AMJ12"/>
+    </row>
+    <row r="13" spans="1:1024" s="6" customFormat="1" ht="24" customHeight="1">
+      <c r="A13" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AMJ12"/>
-    </row>
-    <row r="13" spans="1:1024" s="6" customFormat="1" ht="24" customHeight="1">
-      <c r="A13" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
       <c r="G13" s="18">
         <v>2</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I13" s="12" t="e">
         <f>I12+TIME(0,G13,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="25" t="s">
+      <c r="L13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="M13" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="25" t="s">
+      <c r="N13" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="N13" s="25" t="s">
+      <c r="AMJ13"/>
+    </row>
+    <row r="14" spans="1:1024" s="6" customFormat="1" ht="27" customHeight="1">
+      <c r="A14" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="AMJ13"/>
-    </row>
-    <row r="14" spans="1:1024" s="6" customFormat="1" ht="27" customHeight="1">
-      <c r="A14" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="82"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="84"/>
       <c r="G14" s="18">
         <v>5</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14" s="12" t="e">
         <f>I13+TIME(0,G14,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="K14" s="25" t="s">
+      <c r="L14" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="25" t="s">
+      <c r="M14" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="25" t="s">
         <v>38</v>
-      </c>
-      <c r="M14" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="N14" s="25" t="s">
-        <v>39</v>
       </c>
       <c r="AMJ14"/>
     </row>
@@ -4478,44 +4503,44 @@
         <f>A11+TIME(0,G11,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B15" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
+      <c r="B15" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="15">
         <f>SUM(G16:G20)</f>
         <v>9</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
-      <c r="K15" s="68" t="s">
+      <c r="K15" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="AMJ15"/>
+    </row>
+    <row r="16" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A16" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="68"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="68"/>
-      <c r="AMJ15"/>
-    </row>
-    <row r="16" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A16" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
       <c r="G16" s="18">
         <v>3</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I16" s="12" t="e">
         <f>A15+TIME(0,G16,0)</f>
@@ -4526,185 +4551,185 @@
         <v>{host_name}</v>
       </c>
       <c r="K16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="M16" s="82">
+        <v>18028652848</v>
+      </c>
+      <c r="N16" s="82"/>
+      <c r="AMJ16"/>
+    </row>
+    <row r="17" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A17" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="L16" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="M16" s="80">
-        <v>18028652848</v>
-      </c>
-      <c r="N16" s="80"/>
-      <c r="AMJ16"/>
-    </row>
-    <row r="17" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A17" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
       <c r="G17" s="18">
         <v>1</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I17" s="12" t="e">
         <f>I16+TIME(0,G17,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="L17" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="M17" s="82">
+        <v>13580530646</v>
+      </c>
+      <c r="N17" s="82"/>
+      <c r="AMJ17"/>
+    </row>
+    <row r="18" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A18" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="L17" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="M17" s="80">
-        <v>13580530646</v>
-      </c>
-      <c r="N17" s="80"/>
-      <c r="AMJ17"/>
-    </row>
-    <row r="18" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A18" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
       <c r="G18" s="18">
         <v>1</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" s="12" t="e">
         <f>I17+TIME(0,G18,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J18" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="L18" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M18" s="82">
+        <v>13826106387</v>
+      </c>
+      <c r="N18" s="82"/>
+      <c r="AMJ18"/>
+    </row>
+    <row r="19" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A19" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="M18" s="80">
-        <v>13826106387</v>
-      </c>
-      <c r="N18" s="80"/>
-      <c r="AMJ18"/>
-    </row>
-    <row r="19" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A19" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
       <c r="G19" s="18">
         <v>2</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I19" s="12" t="e">
         <f>I18+TIME(0,G19,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="M19" s="82">
+        <v>17812179178</v>
+      </c>
+      <c r="N19" s="82"/>
+      <c r="AMJ19"/>
+    </row>
+    <row r="20" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A20" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="M19" s="80">
-        <v>17812179178</v>
-      </c>
-      <c r="N19" s="80"/>
-      <c r="AMJ19"/>
-    </row>
-    <row r="20" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A20" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
       <c r="G20" s="18">
         <v>2</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I20" s="12" t="e">
         <f>I19+TIME(0,G20,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="L20" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="M20" s="82">
+        <v>13022004144</v>
+      </c>
+      <c r="N20" s="82"/>
+      <c r="AMJ20"/>
+    </row>
+    <row r="21" spans="1:1024" s="4" customFormat="1" ht="27" customHeight="1">
+      <c r="A21" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="L20" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="M20" s="80">
-        <v>13022004144</v>
-      </c>
-      <c r="N20" s="80"/>
-      <c r="AMJ20"/>
-    </row>
-    <row r="21" spans="1:1024" s="4" customFormat="1" ht="27" customHeight="1">
-      <c r="A21" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
       <c r="G21" s="18">
         <v>6</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I21" s="12" t="e">
         <f>I20+TIME(0,G21,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J21" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="L21" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="M21" s="80">
+        <v>154</v>
+      </c>
+      <c r="M21" s="82">
         <v>15920428594</v>
       </c>
-      <c r="N21" s="80"/>
+      <c r="N21" s="82"/>
       <c r="AMJ21"/>
     </row>
     <row r="22" spans="1:1024" s="4" customFormat="1" ht="27" customHeight="1">
@@ -4712,170 +4737,170 @@
         <f>A15+TIME(0,G15,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B22" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
+      <c r="B22" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
       <c r="G22" s="15">
         <f>SUM(G23:G27)</f>
         <v>29</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
       <c r="K22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="M22" s="82">
+        <v>15918836991</v>
+      </c>
+      <c r="N22" s="82"/>
+      <c r="AMJ22"/>
+    </row>
+    <row r="23" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A23" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="L22" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="M22" s="80">
-        <v>15918836991</v>
-      </c>
-      <c r="N22" s="80"/>
-      <c r="AMJ22"/>
-    </row>
-    <row r="23" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A23" s="65" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
       <c r="G23" s="18">
         <v>1</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I23" s="12" t="e">
         <f>A22+TIME(0,G23,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K23" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="M23" s="82">
+        <v>13826106387</v>
+      </c>
+      <c r="N23" s="82"/>
+      <c r="AMJ23"/>
+    </row>
+    <row r="24" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A24" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="L23" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="M23" s="80">
-        <v>13826106387</v>
-      </c>
-      <c r="N23" s="80"/>
-      <c r="AMJ23"/>
-    </row>
-    <row r="24" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A24" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
       <c r="G24" s="18">
         <v>2</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I24" s="12" t="e">
         <f>I23+TIME(0,G24,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K24" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="L24" s="70"/>
-      <c r="M24" s="70"/>
-      <c r="N24" s="70"/>
+        <v>35</v>
+      </c>
+      <c r="K24" s="83" t="s">
+        <v>164</v>
+      </c>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
       <c r="AMJ24"/>
     </row>
     <row r="25" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A25" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
+      <c r="A25" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
       <c r="G25" s="18">
         <v>18</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I25" s="12" t="e">
         <f>I24+TIME(0,G25,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="K25" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="L25" s="75"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="76"/>
+        <v>63</v>
+      </c>
+      <c r="K25" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="L25" s="74"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="75"/>
       <c r="AMJ25"/>
     </row>
     <row r="26" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A26" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
+      <c r="A26" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
       <c r="G26" s="28">
         <v>7</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I26" s="12" t="e">
         <f>I25+TIME(0,G26,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="K26" s="77"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="79"/>
+        <v>65</v>
+      </c>
+      <c r="K26" s="76"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="78"/>
       <c r="AMJ26"/>
     </row>
     <row r="27" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A27" s="65" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
+      <c r="A27" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
       <c r="G27" s="28">
         <v>1</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I27" s="12" t="e">
         <f>I26+TIME(0,G27,0)</f>
@@ -4885,10 +4910,10 @@
         <f>J12</f>
         <v>{host_name}</v>
       </c>
-      <c r="K27" s="55"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="55"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="80"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="81"/>
       <c r="AMJ27"/>
     </row>
     <row r="28" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
@@ -4896,42 +4921,42 @@
         <f>A22+TIME(0,G22,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B28" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
+      <c r="B28" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
       <c r="G28" s="15">
         <f>SUM(G29:G35)</f>
         <v>25</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="73"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
+        <v>20</v>
+      </c>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
       <c r="AMJ28"/>
     </row>
     <row r="29" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A29" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
+      <c r="A29" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
       <c r="G29" s="18">
         <v>1</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I29" s="30" t="e">
         <f>A28+TIME(0,G29,0)</f>
@@ -4941,54 +4966,54 @@
         <f>J12</f>
         <v>{host_name}</v>
       </c>
-      <c r="K29" s="55"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51"/>
       <c r="AMJ29"/>
     </row>
     <row r="30" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A30" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
+      <c r="A30" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
       <c r="G30" s="18">
         <v>7</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I30" s="30" t="e">
         <f t="shared" ref="I30:I35" si="0">I29+TIME(0,G30,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="K30" s="55"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="55"/>
+        <v>68</v>
+      </c>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
       <c r="AMJ30"/>
     </row>
     <row r="31" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A31" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
+      <c r="A31" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
       <c r="G31" s="18">
         <v>1</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I31" s="30" t="e">
         <f t="shared" si="0"/>
@@ -4998,56 +5023,56 @@
         <f>J29</f>
         <v>{host_name}</v>
       </c>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="55"/>
-      <c r="N31" s="55"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
       <c r="AMJ31"/>
     </row>
     <row r="32" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A32" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
+      <c r="A32" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
       <c r="G32" s="18">
         <v>7</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I32" s="30" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="K32" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="L32" s="70"/>
-      <c r="M32" s="70"/>
-      <c r="N32" s="70"/>
+        <v>70</v>
+      </c>
+      <c r="K32" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
       <c r="AMJ32"/>
     </row>
     <row r="33" spans="1:1024" s="4" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A33" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
+      <c r="A33" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
       <c r="G33" s="18">
         <v>1</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I33" s="30" t="e">
         <f t="shared" si="0"/>
@@ -5057,56 +5082,56 @@
         <f>J12</f>
         <v>{host_name}</v>
       </c>
-      <c r="K33" s="71" t="s">
-        <v>165</v>
-      </c>
-      <c r="L33" s="72"/>
-      <c r="M33" s="72"/>
-      <c r="N33" s="72"/>
+      <c r="K33" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="71"/>
       <c r="AMJ33"/>
     </row>
     <row r="34" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A34" s="69" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
+      <c r="A34" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
       <c r="G34" s="28">
         <v>7</v>
       </c>
       <c r="H34" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I34" s="32" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="J34" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="K34" s="72"/>
-      <c r="L34" s="72"/>
-      <c r="M34" s="72"/>
-      <c r="N34" s="72"/>
+        <v>73</v>
+      </c>
+      <c r="K34" s="71"/>
+      <c r="L34" s="71"/>
+      <c r="M34" s="71"/>
+      <c r="N34" s="71"/>
       <c r="AMJ34"/>
     </row>
     <row r="35" spans="1:1024" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A35" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="65"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
+      <c r="A35" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
       <c r="G35" s="18">
         <v>1</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I35" s="30" t="e">
         <f t="shared" si="0"/>
@@ -5116,10 +5141,10 @@
         <f>J29</f>
         <v>{host_name}</v>
       </c>
-      <c r="K35" s="72"/>
-      <c r="L35" s="72"/>
-      <c r="M35" s="72"/>
-      <c r="N35" s="72"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="71"/>
+      <c r="N35" s="71"/>
       <c r="AMJ35"/>
     </row>
     <row r="36" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
@@ -5127,25 +5152,25 @@
         <f>A28+TIME(0,G28,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B36" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
+      <c r="B36" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="15">
         <v>5</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="72"/>
-      <c r="M36" s="72"/>
-      <c r="N36" s="72"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="71"/>
+      <c r="N36" s="71"/>
       <c r="AMJ36"/>
     </row>
     <row r="37" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
@@ -5153,42 +5178,42 @@
         <f>A36+TIME(0,G36,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B37" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
+      <c r="B37" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="15">
         <f>SUM(G38:G41)</f>
         <v>10</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="72"/>
-      <c r="M37" s="72"/>
-      <c r="N37" s="72"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
+      <c r="N37" s="71"/>
       <c r="AMJ37"/>
     </row>
     <row r="38" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A38" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
+      <c r="A38" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
       <c r="G38" s="18">
         <v>1</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I38" s="30" t="e">
         <f>A37+TIME(0,G38,0)</f>
@@ -5198,98 +5223,98 @@
         <f>J12</f>
         <v>{host_name}</v>
       </c>
-      <c r="K38" s="72"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="72"/>
-      <c r="N38" s="72"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
+      <c r="N38" s="71"/>
       <c r="AMJ38"/>
     </row>
     <row r="39" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A39" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="69"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
+      <c r="A39" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="68"/>
       <c r="G39" s="18">
         <v>3</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I39" s="30" t="e">
         <f>I38+TIME(0,G39,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="72"/>
-      <c r="N39" s="72"/>
+        <v>52</v>
+      </c>
+      <c r="K39" s="71"/>
+      <c r="L39" s="71"/>
+      <c r="M39" s="71"/>
+      <c r="N39" s="71"/>
       <c r="AMJ39"/>
     </row>
     <row r="40" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A40" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="65"/>
+      <c r="A40" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
       <c r="G40" s="18">
         <v>3</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I40" s="30" t="e">
         <f>I39+TIME(0,G40,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="K40" s="72"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="72"/>
-      <c r="N40" s="72"/>
+        <v>78</v>
+      </c>
+      <c r="K40" s="71"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
+      <c r="N40" s="71"/>
       <c r="AMJ40"/>
     </row>
     <row r="41" spans="1:1024" s="4" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A41" s="69" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="69"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
+      <c r="A41" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
       <c r="G41" s="18">
         <v>3</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I41" s="30" t="e">
         <f>I40+TIME(0,G41,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="K41" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="L41" s="70"/>
-      <c r="M41" s="70"/>
-      <c r="N41" s="70"/>
+        <v>80</v>
+      </c>
+      <c r="K41" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="L41" s="69"/>
+      <c r="M41" s="69"/>
+      <c r="N41" s="69"/>
       <c r="O41" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AMJ41"/>
     </row>
@@ -5298,47 +5323,47 @@
         <f>A37+TIME(0,G37,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B42" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
+      <c r="B42" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
       <c r="G42" s="15">
         <f>SUM(G43:G47)</f>
         <v>15</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="L42" s="62"/>
-      <c r="M42" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="N42" s="62"/>
+      <c r="K42" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="L42" s="61"/>
+      <c r="M42" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="N42" s="61"/>
       <c r="O42" s="7"/>
       <c r="AMJ42"/>
     </row>
     <row r="43" spans="1:1024" s="4" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A43" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
-      <c r="F43" s="64"/>
+      <c r="A43" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="63"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="63"/>
       <c r="G43" s="18">
         <v>1</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I43" s="12" t="e">
         <f>A42+TIME(0,G43,0)</f>
@@ -5348,31 +5373,31 @@
         <f>J16</f>
         <v>{host_name}</v>
       </c>
-      <c r="K43" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="L43" s="62"/>
-      <c r="M43" s="62" t="s">
-        <v>91</v>
-      </c>
-      <c r="N43" s="62"/>
+      <c r="K43" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="L43" s="61"/>
+      <c r="M43" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="N43" s="61"/>
       <c r="O43" s="7"/>
       <c r="AMJ43"/>
     </row>
     <row r="44" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A44" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
+      <c r="A44" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
       <c r="G44" s="18">
         <v>2</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I44" s="12" t="e">
         <f>I43+TIME(0,G44,0)</f>
@@ -5382,30 +5407,30 @@
         <f>J17</f>
         <v>丘愉庄</v>
       </c>
-      <c r="K44" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="L44" s="62"/>
-      <c r="M44" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="N44" s="62"/>
+      <c r="K44" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="L44" s="61"/>
+      <c r="M44" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="N44" s="61"/>
       <c r="AMJ44"/>
     </row>
     <row r="45" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A45" s="64" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
+      <c r="A45" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="63"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
       <c r="G45" s="18">
         <v>2</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I45" s="12" t="e">
         <f>I44+TIME(0,G45,0)</f>
@@ -5415,30 +5440,30 @@
         <f>J18</f>
         <v>xxx</v>
       </c>
-      <c r="K45" s="62" t="s">
-        <v>96</v>
-      </c>
-      <c r="L45" s="62"/>
-      <c r="M45" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="N45" s="62"/>
+      <c r="K45" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="L45" s="61"/>
+      <c r="M45" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="N45" s="61"/>
       <c r="AMJ45"/>
     </row>
     <row r="46" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A46" s="64" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" s="64"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
+      <c r="A46" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="63"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
       <c r="G46" s="18">
         <v>3</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I46" s="12" t="e">
         <f>I45+TIME(0,G46,0)</f>
@@ -5448,69 +5473,69 @@
         <f>J19</f>
         <v>xxx</v>
       </c>
-      <c r="K46" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="L46" s="62"/>
-      <c r="M46" s="62" t="s">
-        <v>100</v>
-      </c>
-      <c r="N46" s="62"/>
+      <c r="K46" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="L46" s="61"/>
+      <c r="M46" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="N46" s="61"/>
       <c r="AMJ46"/>
     </row>
     <row r="47" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A47" s="64" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="64"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
+      <c r="A47" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
       <c r="G47" s="18">
         <v>7</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I47" s="12" t="e">
         <f>I46+TIME(0,G47,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K47" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="L47" s="62"/>
-      <c r="M47" s="66"/>
-      <c r="N47" s="66"/>
+        <v>52</v>
+      </c>
+      <c r="K47" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="L47" s="61"/>
+      <c r="M47" s="65"/>
+      <c r="N47" s="65"/>
       <c r="AMJ47"/>
     </row>
     <row r="48" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
       <c r="A48" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="66"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="66"/>
+      <c r="I48" s="66"/>
+      <c r="J48" s="66"/>
+      <c r="K48" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="L48" s="67"/>
+      <c r="M48" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="67"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="67"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="67"/>
-      <c r="I48" s="67"/>
-      <c r="J48" s="67"/>
-      <c r="K48" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="L48" s="68"/>
-      <c r="M48" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="N48" s="68"/>
+      <c r="N48" s="67"/>
       <c r="AMJ48"/>
     </row>
     <row r="49" spans="1:1024" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -5518,127 +5543,127 @@
         <f>A42+TIME(0,G42,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B49" s="61" t="s">
-        <v>107</v>
-      </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
+      <c r="B49" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="60"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
       <c r="G49" s="15">
         <f>SUM(G50:G52)</f>
         <v>8</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="17"/>
-      <c r="K49" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="L49" s="62"/>
-      <c r="M49" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="N49" s="62"/>
+      <c r="K49" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="L49" s="61"/>
+      <c r="M49" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="N49" s="61"/>
       <c r="AMJ49"/>
     </row>
     <row r="50" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A50" s="65" t="s">
-        <v>110</v>
-      </c>
-      <c r="B50" s="65"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="65"/>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
+      <c r="A50" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="64"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
       <c r="G50" s="28">
         <v>4</v>
       </c>
       <c r="H50" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I50" s="34" t="e">
         <f>A49+TIME(0,G50,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K50" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="L50" s="62"/>
-      <c r="M50" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="N50" s="62"/>
+        <v>29</v>
+      </c>
+      <c r="K50" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="L50" s="61"/>
+      <c r="M50" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="N50" s="61"/>
       <c r="AMJ50"/>
     </row>
     <row r="51" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A51" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
+      <c r="A51" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
       <c r="G51" s="18">
         <v>3</v>
       </c>
       <c r="H51" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I51" s="12" t="e">
         <f>I50+TIME(0,G51,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K51" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="L51" s="62"/>
-      <c r="M51" s="62" t="s">
-        <v>115</v>
-      </c>
-      <c r="N51" s="62"/>
+        <v>29</v>
+      </c>
+      <c r="K51" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="L51" s="61"/>
+      <c r="M51" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="N51" s="61"/>
       <c r="AMJ51"/>
     </row>
     <row r="52" spans="1:1024" s="4" customFormat="1" ht="19.350000000000001" customHeight="1">
-      <c r="A52" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="B52" s="64"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
+      <c r="A52" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="63"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="63"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="63"/>
       <c r="G52" s="18">
         <v>1</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I52" s="12" t="e">
         <f>I51+TIME(0,G52,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="K52" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="L52" s="62"/>
-      <c r="M52" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="N52" s="62"/>
-      <c r="O52" s="59"/>
+        <v>114</v>
+      </c>
+      <c r="K52" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="L52" s="61"/>
+      <c r="M52" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="N52" s="61"/>
+      <c r="O52" s="58"/>
       <c r="AMJ52"/>
     </row>
     <row r="53" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
@@ -5646,30 +5671,30 @@
         <f>A49+TIME(0,G49,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B53" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
-      <c r="H53" s="61"/>
-      <c r="I53" s="61"/>
-      <c r="J53" s="61"/>
-      <c r="K53" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="L53" s="62"/>
-      <c r="M53" s="62" t="s">
-        <v>122</v>
-      </c>
-      <c r="N53" s="62"/>
-      <c r="O53" s="59"/>
+      <c r="B53" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="60"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="L53" s="61"/>
+      <c r="M53" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="N53" s="61"/>
+      <c r="O53" s="58"/>
       <c r="AMJ53"/>
     </row>
     <row r="54" spans="1:1024" ht="24" customHeight="1">
-      <c r="O54" s="60"/>
+      <c r="O54" s="59"/>
     </row>
     <row r="55" spans="1:1024" ht="24" customHeight="1"/>
     <row r="56" spans="1:1024" ht="24" customHeight="1"/>
@@ -5684,13 +5709,14 @@
     <row r="1048575" ht="12.75" customHeight="1"/>
     <row r="1048576" ht="12.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="94">
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="D2:M2"/>
+  <mergeCells count="95">
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="B8:H8"/>
     <mergeCell ref="K8:N8"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="N1:N3"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="K9:N10"/>
@@ -5714,6 +5740,7 @@
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="M21:N21"/>
+    <mergeCell ref="K25:N27"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="A23:F23"/>
@@ -5723,7 +5750,6 @@
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A27:F27"/>
-    <mergeCell ref="K25:N26"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="A29:F29"/>
@@ -5780,7 +5806,7 @@
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="M52:N52"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="6.9444444444444406E-2" top="0.6" bottom="0.65972222222222199" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" scale="60" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5790,10 +5816,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5803,124 +5829,116 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>

<commit_message>
allowing parse and write multiple line content
</commit_message>
<xml_diff>
--- a/example/jabil_jouse_template_for_print/jabil_jouse_template_for_print.xlsx
+++ b/example/jabil_jouse_template_for_print/jabil_jouse_template_for_print.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\头马会议经理文件包\tmma_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2669E6B1-D961-4238-9D3B-82FCA9E86C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5B220E-00EA-4E4C-AE7B-C5C1C1C3B3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="copy">#REF!</definedName>
     <definedName name="dfdsf" localSheetId="0">#REF!</definedName>
     <definedName name="dfdsf">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">template!$A$1:$N$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">template!$A$1:$N$53</definedName>
     <definedName name="qwertyu">#REF!</definedName>
     <definedName name="对he_chun_qing《李广难封》的备稿演讲点评">#REF!</definedName>
   </definedNames>
@@ -39,37 +39,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="24"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>会议标题</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="10"/>
         <rFont val="宋体"/>
         <family val="2"/>
@@ -123,46 +92,12 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>线上会议号</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>}</t>
-    </r>
-  </si>
-  <si>
     <t>摄影师：{摄影师}</t>
   </si>
   <si>
     <t xml:space="preserve">时间 </t>
   </si>
   <si>
-    <t>主题：{主题}</t>
-  </si>
-  <si>
     <t>时间</t>
   </si>
   <si>
@@ -172,63 +107,7 @@
     <t>会议规定</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>开始时间</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>}</t>
-    </r>
-  </si>
-  <si>
     <t>会议组织者</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>开始时间</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">} </t>
-    </r>
   </si>
   <si>
     <t>{会议经理}</t>
@@ -1830,34 +1709,30 @@
   </si>
   <si>
     <t>林长宏（Leon Lin）</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>丘愉庄（Rainbow Qiu）</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>黎泳恩（Vivian Li)</t>
   </si>
   <si>
     <t>刘惠芳（Annie Liu）</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>N26</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>捷普聚思国际演讲俱乐部</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>（俱乐部号：5614337）</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>张合堂（Hunter Zhang）</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1946,7 +1821,7 @@
       </rPr>
       <t>）。</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1961,11 +1836,41 @@
       </rPr>
       <t>时间：</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>线上：</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>备稿演讲项目简介</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>会议标题%第319次线下中文会议</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1978,7 +1883,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>日期</t>
+      <t>日期%2023年7月21日</t>
     </r>
     <r>
       <rPr>
@@ -1989,11 +1894,106 @@
       </rPr>
       <t>}</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>备稿演讲项目简介</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开始时间%15:00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{开始时间%15:00}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>主题：</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>主题%旅行</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线上会议号%123-456-8987</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>N27</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2006,7 +2006,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>备稿演讲项目简介</t>
+      <t>备稿演讲项目简介%</t>
     </r>
     <r>
       <rPr>
@@ -2014,9 +2014,72 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">L1P1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">初试啼声，介绍自己
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">L2P1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>演讲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>项目</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内容</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>}</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2026,7 +2089,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2052,12 +2115,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2079,12 +2136,6 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2248,6 +2299,46 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -2293,7 +2384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2409,16 +2500,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2431,164 +2535,284 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="27" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="18" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="29" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="20" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2597,125 +2821,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3752,7 +3859,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>481740</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>27180</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3786,16 +3893,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>777240</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
+      <xdr:colOff>988695</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>58420</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3818,7 +3925,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8549640" y="7620"/>
+          <a:off x="8595360" y="22860"/>
           <a:ext cx="950595" cy="919480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4132,10 +4239,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4159,47 +4269,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="37.200000000000003">
-      <c r="A1" s="93"/>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="90" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
       <c r="K1" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L1" s="53"/>
       <c r="M1" s="53"/>
-      <c r="N1" s="98"/>
-    </row>
-    <row r="2" spans="1:1024" ht="31.2">
-      <c r="A2" s="95"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
+      <c r="N1" s="71"/>
+    </row>
+    <row r="2" spans="1:1024" ht="33">
+      <c r="A2" s="68"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
       <c r="K2" s="57"/>
       <c r="L2" s="57"/>
       <c r="M2" s="57"/>
-      <c r="N2" s="99"/>
+      <c r="N2" s="72"/>
     </row>
     <row r="3" spans="1:1024" s="4" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
       <c r="D3" s="37"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -4208,21 +4318,21 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="38"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="99"/>
+      <c r="N3" s="72"/>
       <c r="AMJ3"/>
     </row>
     <row r="4" spans="1:1024" s="4" customFormat="1" ht="15.6" customHeight="1">
       <c r="A4" s="55"/>
       <c r="B4" s="56"/>
       <c r="D4" s="37" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="1"/>
@@ -4230,21 +4340,21 @@
       <c r="I4" s="3"/>
       <c r="J4" s="40"/>
       <c r="K4" s="38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="38"/>
       <c r="N4" s="43"/>
       <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1024" s="4" customFormat="1" ht="15.6">
-      <c r="A5" s="88" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
+    <row r="5" spans="1:1024" s="4" customFormat="1" ht="16.2">
+      <c r="A5" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
       <c r="E5" s="41" t="s">
-        <v>3</v>
+        <v>163</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
@@ -4265,7 +4375,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="L6" s="42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N6" s="43"/>
       <c r="AMJ6"/>
@@ -4289,212 +4399,212 @@
     </row>
     <row r="8" spans="1:1024" s="5" customFormat="1" ht="24" customHeight="1">
       <c r="A8" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="K8" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="36" t="s">
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="AMJ8"/>
+    </row>
+    <row r="9" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A9" s="73" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="92" t="s">
+      <c r="K9" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="92"/>
-      <c r="AMJ8"/>
-    </row>
-    <row r="9" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A9" s="85" t="s">
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="AMJ9"/>
+    </row>
+    <row r="10" spans="1:1024" s="4" customFormat="1" ht="22.8" customHeight="1">
+      <c r="A10" s="74"/>
+      <c r="B10" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="J10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="86" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="AMJ9"/>
-    </row>
-    <row r="10" spans="1:1024" s="4" customFormat="1" ht="22.8" customHeight="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="84" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" s="4" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="87" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
+        <v>12</v>
+      </c>
+      <c r="B11" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
       <c r="G11" s="15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
-      <c r="K11" s="67" t="s">
+      <c r="K11" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
+      <c r="AMJ11"/>
+    </row>
+    <row r="12" spans="1:1024" s="6" customFormat="1" ht="24" customHeight="1">
+      <c r="A12" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="AMJ11"/>
-    </row>
-    <row r="12" spans="1:1024" s="6" customFormat="1" ht="24" customHeight="1">
-      <c r="A12" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="12" t="s">
+      <c r="N12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="AMJ12"/>
+    </row>
+    <row r="13" spans="1:1024" s="6" customFormat="1" ht="24" customHeight="1">
+      <c r="A13" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="AMJ12"/>
-    </row>
-    <row r="13" spans="1:1024" s="6" customFormat="1" ht="24" customHeight="1">
-      <c r="A13" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
       <c r="G13" s="18">
         <v>2</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I13" s="12" t="e">
         <f>I12+TIME(0,G13,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AMJ13"/>
+    </row>
+    <row r="14" spans="1:1024" s="6" customFormat="1" ht="27" customHeight="1">
+      <c r="A14" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="AMJ13"/>
-    </row>
-    <row r="14" spans="1:1024" s="6" customFormat="1" ht="27" customHeight="1">
-      <c r="A14" s="84" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
       <c r="G14" s="18">
         <v>5</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I14" s="12" t="e">
         <f>I13+TIME(0,G14,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="M14" s="25" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="N14" s="25" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="AMJ14"/>
     </row>
@@ -4503,44 +4613,44 @@
         <f>A11+TIME(0,G11,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B15" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
+      <c r="B15" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
       <c r="G15" s="15">
         <f>SUM(G16:G20)</f>
         <v>9</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
-      <c r="K15" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
+      <c r="K15" s="79" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
       <c r="AMJ15"/>
     </row>
     <row r="16" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A16" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
+      <c r="A16" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
       <c r="G16" s="18">
         <v>3</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I16" s="12" t="e">
         <f>A15+TIME(0,G16,0)</f>
@@ -4551,185 +4661,185 @@
         <v>{host_name}</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="M16" s="82">
+        <v>144</v>
+      </c>
+      <c r="M16" s="81">
         <v>18028652848</v>
       </c>
-      <c r="N16" s="82"/>
+      <c r="N16" s="81"/>
       <c r="AMJ16"/>
     </row>
     <row r="17" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A17" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
+      <c r="A17" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
       <c r="G17" s="18">
         <v>1</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I17" s="12" t="e">
         <f>I16+TIME(0,G17,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="M17" s="82">
+        <v>145</v>
+      </c>
+      <c r="M17" s="81">
         <v>13580530646</v>
       </c>
-      <c r="N17" s="82"/>
+      <c r="N17" s="81"/>
       <c r="AMJ17"/>
     </row>
     <row r="18" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A18" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
+      <c r="A18" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
       <c r="G18" s="18">
         <v>1</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I18" s="12" t="e">
         <f>I17+TIME(0,G18,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J18" s="26" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="M18" s="82">
+        <v>146</v>
+      </c>
+      <c r="M18" s="81">
         <v>13826106387</v>
       </c>
-      <c r="N18" s="82"/>
+      <c r="N18" s="81"/>
       <c r="AMJ18"/>
     </row>
     <row r="19" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A19" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
+      <c r="A19" s="82" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
       <c r="G19" s="18">
         <v>2</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I19" s="12" t="e">
         <f>I18+TIME(0,G19,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="M19" s="82">
+        <v>147</v>
+      </c>
+      <c r="M19" s="81">
         <v>17812179178</v>
       </c>
-      <c r="N19" s="82"/>
+      <c r="N19" s="81"/>
       <c r="AMJ19"/>
     </row>
     <row r="20" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A20" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
+      <c r="A20" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
       <c r="G20" s="18">
         <v>2</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I20" s="12" t="e">
         <f>I19+TIME(0,G20,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="M20" s="82">
+        <v>148</v>
+      </c>
+      <c r="M20" s="81">
         <v>13022004144</v>
       </c>
-      <c r="N20" s="82"/>
+      <c r="N20" s="81"/>
       <c r="AMJ20"/>
     </row>
     <row r="21" spans="1:1024" s="4" customFormat="1" ht="27" customHeight="1">
-      <c r="A21" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
+      <c r="A21" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
       <c r="G21" s="18">
         <v>6</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I21" s="12" t="e">
         <f>I20+TIME(0,G21,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="M21" s="82">
+        <v>149</v>
+      </c>
+      <c r="M21" s="81">
         <v>15920428594</v>
       </c>
-      <c r="N21" s="82"/>
+      <c r="N21" s="81"/>
       <c r="AMJ21"/>
     </row>
     <row r="22" spans="1:1024" s="4" customFormat="1" ht="27" customHeight="1">
@@ -4737,170 +4847,170 @@
         <f>A15+TIME(0,G15,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B22" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
+      <c r="B22" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
       <c r="G22" s="15">
         <f>SUM(G23:G27)</f>
         <v>29</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
       <c r="K22" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="M22" s="82">
+        <v>150</v>
+      </c>
+      <c r="M22" s="81">
         <v>15918836991</v>
       </c>
-      <c r="N22" s="82"/>
+      <c r="N22" s="81"/>
       <c r="AMJ22"/>
     </row>
     <row r="23" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A23" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
+      <c r="A23" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
       <c r="G23" s="18">
         <v>1</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I23" s="12" t="e">
         <f>A22+TIME(0,G23,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="K23" s="27" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="M23" s="82">
+        <v>153</v>
+      </c>
+      <c r="M23" s="81">
         <v>13826106387</v>
       </c>
-      <c r="N23" s="82"/>
+      <c r="N23" s="81"/>
       <c r="AMJ23"/>
     </row>
     <row r="24" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A24" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
+      <c r="A24" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
       <c r="G24" s="18">
         <v>2</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I24" s="12" t="e">
         <f>I23+TIME(0,G24,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K24" s="83" t="s">
-        <v>164</v>
-      </c>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
+        <v>30</v>
+      </c>
+      <c r="K24" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="L24" s="91"/>
+      <c r="M24" s="91"/>
+      <c r="N24" s="91"/>
       <c r="AMJ24"/>
     </row>
     <row r="25" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A25" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
+      <c r="A25" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
       <c r="G25" s="18">
         <v>18</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I25" s="12" t="e">
         <f>I24+TIME(0,G25,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K25" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="K25" s="83" t="s">
         <v>165</v>
       </c>
-      <c r="L25" s="74"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="75"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="84"/>
+      <c r="N25" s="85"/>
       <c r="AMJ25"/>
     </row>
     <row r="26" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A26" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
+      <c r="A26" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
       <c r="G26" s="28">
         <v>7</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I26" s="12" t="e">
         <f>I25+TIME(0,G26,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="K26" s="76"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="78"/>
+        <v>60</v>
+      </c>
+      <c r="K26" s="86"/>
+      <c r="L26" s="87"/>
+      <c r="M26" s="87"/>
+      <c r="N26" s="88"/>
       <c r="AMJ26"/>
     </row>
     <row r="27" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A27" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
+      <c r="A27" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
       <c r="G27" s="28">
         <v>1</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I27" s="12" t="e">
         <f>I26+TIME(0,G27,0)</f>
@@ -4910,10 +5020,10 @@
         <f>J12</f>
         <v>{host_name}</v>
       </c>
-      <c r="K27" s="79"/>
-      <c r="L27" s="80"/>
-      <c r="M27" s="80"/>
-      <c r="N27" s="81"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="88"/>
       <c r="AMJ27"/>
     </row>
     <row r="28" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
@@ -4921,42 +5031,42 @@
         <f>A22+TIME(0,G22,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B28" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
+      <c r="B28" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
       <c r="G28" s="15">
         <f>SUM(G29:G35)</f>
         <v>25</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
+        <v>15</v>
+      </c>
+      <c r="I28" s="92"/>
+      <c r="J28" s="92"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
       <c r="AMJ28"/>
     </row>
     <row r="29" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A29" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
+      <c r="A29" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="89"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
       <c r="G29" s="18">
         <v>1</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I29" s="30" t="e">
         <f>A28+TIME(0,G29,0)</f>
@@ -4973,26 +5083,26 @@
       <c r="AMJ29"/>
     </row>
     <row r="30" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A30" s="68" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
+      <c r="A30" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
       <c r="G30" s="18">
         <v>7</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I30" s="30" t="e">
         <f t="shared" ref="I30:I35" si="0">I29+TIME(0,G30,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K30" s="51"/>
       <c r="L30" s="51"/>
@@ -5001,19 +5111,19 @@
       <c r="AMJ30"/>
     </row>
     <row r="31" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A31" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
+      <c r="A31" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
       <c r="G31" s="18">
         <v>1</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I31" s="30" t="e">
         <f t="shared" si="0"/>
@@ -5030,49 +5140,49 @@
       <c r="AMJ31"/>
     </row>
     <row r="32" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A32" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
+      <c r="A32" s="89" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
       <c r="G32" s="18">
         <v>7</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I32" s="30" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="K32" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="69"/>
+        <v>65</v>
+      </c>
+      <c r="K32" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="L32" s="91"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="91"/>
       <c r="AMJ32"/>
     </row>
     <row r="33" spans="1:1024" s="4" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A33" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
+      <c r="A33" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="89"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
       <c r="G33" s="18">
         <v>1</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I33" s="30" t="e">
         <f t="shared" si="0"/>
@@ -5082,56 +5192,56 @@
         <f>J12</f>
         <v>{host_name}</v>
       </c>
-      <c r="K33" s="70" t="s">
-        <v>160</v>
-      </c>
-      <c r="L33" s="71"/>
-      <c r="M33" s="71"/>
-      <c r="N33" s="71"/>
+      <c r="K33" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
       <c r="AMJ33"/>
     </row>
     <row r="34" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A34" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
+      <c r="A34" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
       <c r="G34" s="28">
         <v>7</v>
       </c>
       <c r="H34" s="31" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I34" s="32" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="J34" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="K34" s="71"/>
-      <c r="L34" s="71"/>
-      <c r="M34" s="71"/>
-      <c r="N34" s="71"/>
+        <v>68</v>
+      </c>
+      <c r="K34" s="94"/>
+      <c r="L34" s="94"/>
+      <c r="M34" s="94"/>
+      <c r="N34" s="94"/>
       <c r="AMJ34"/>
     </row>
     <row r="35" spans="1:1024" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A35" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="64"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
+      <c r="A35" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
       <c r="G35" s="18">
         <v>1</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I35" s="30" t="e">
         <f t="shared" si="0"/>
@@ -5141,10 +5251,10 @@
         <f>J29</f>
         <v>{host_name}</v>
       </c>
-      <c r="K35" s="71"/>
-      <c r="L35" s="71"/>
-      <c r="M35" s="71"/>
-      <c r="N35" s="71"/>
+      <c r="K35" s="94"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="94"/>
       <c r="AMJ35"/>
     </row>
     <row r="36" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
@@ -5152,25 +5262,25 @@
         <f>A28+TIME(0,G28,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B36" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="60"/>
+      <c r="B36" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
       <c r="G36" s="15">
         <v>5</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
-      <c r="K36" s="71"/>
-      <c r="L36" s="71"/>
-      <c r="M36" s="71"/>
-      <c r="N36" s="71"/>
+      <c r="K36" s="94"/>
+      <c r="L36" s="94"/>
+      <c r="M36" s="94"/>
+      <c r="N36" s="94"/>
       <c r="AMJ36"/>
     </row>
     <row r="37" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
@@ -5178,42 +5288,42 @@
         <f>A36+TIME(0,G36,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B37" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="B37" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
       <c r="G37" s="15">
         <f>SUM(G38:G41)</f>
         <v>10</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
-      <c r="K37" s="71"/>
-      <c r="L37" s="71"/>
-      <c r="M37" s="71"/>
-      <c r="N37" s="71"/>
+      <c r="K37" s="94"/>
+      <c r="L37" s="94"/>
+      <c r="M37" s="94"/>
+      <c r="N37" s="94"/>
       <c r="AMJ37"/>
     </row>
     <row r="38" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A38" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="64"/>
+      <c r="A38" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="89"/>
       <c r="G38" s="18">
         <v>1</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I38" s="30" t="e">
         <f>A37+TIME(0,G38,0)</f>
@@ -5223,98 +5333,98 @@
         <f>J12</f>
         <v>{host_name}</v>
       </c>
-      <c r="K38" s="71"/>
-      <c r="L38" s="71"/>
-      <c r="M38" s="71"/>
-      <c r="N38" s="71"/>
+      <c r="K38" s="94"/>
+      <c r="L38" s="94"/>
+      <c r="M38" s="94"/>
+      <c r="N38" s="94"/>
       <c r="AMJ38"/>
     </row>
     <row r="39" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A39" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
+      <c r="A39" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
       <c r="G39" s="18">
         <v>3</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I39" s="30" t="e">
         <f>I38+TIME(0,G39,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K39" s="71"/>
-      <c r="L39" s="71"/>
-      <c r="M39" s="71"/>
-      <c r="N39" s="71"/>
+        <v>47</v>
+      </c>
+      <c r="K39" s="94"/>
+      <c r="L39" s="94"/>
+      <c r="M39" s="94"/>
+      <c r="N39" s="94"/>
       <c r="AMJ39"/>
     </row>
     <row r="40" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A40" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="64"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="64"/>
+      <c r="A40" s="89" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
       <c r="G40" s="18">
         <v>3</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I40" s="30" t="e">
         <f>I39+TIME(0,G40,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="K40" s="71"/>
-      <c r="L40" s="71"/>
-      <c r="M40" s="71"/>
-      <c r="N40" s="71"/>
+        <v>73</v>
+      </c>
+      <c r="K40" s="94"/>
+      <c r="L40" s="94"/>
+      <c r="M40" s="94"/>
+      <c r="N40" s="94"/>
       <c r="AMJ40"/>
     </row>
     <row r="41" spans="1:1024" s="4" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A41" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="68"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
+      <c r="A41" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="82"/>
+      <c r="C41" s="82"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="82"/>
+      <c r="F41" s="82"/>
       <c r="G41" s="18">
         <v>3</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I41" s="30" t="e">
         <f>I40+TIME(0,G41,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="K41" s="69" t="s">
-        <v>81</v>
-      </c>
-      <c r="L41" s="69"/>
-      <c r="M41" s="69"/>
-      <c r="N41" s="69"/>
+        <v>75</v>
+      </c>
+      <c r="K41" s="91" t="s">
+        <v>76</v>
+      </c>
+      <c r="L41" s="91"/>
+      <c r="M41" s="91"/>
+      <c r="N41" s="91"/>
       <c r="O41" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="AMJ41"/>
     </row>
@@ -5323,47 +5433,47 @@
         <f>A37+TIME(0,G37,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B42" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
+      <c r="B42" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="80"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="80"/>
+      <c r="F42" s="80"/>
       <c r="G42" s="15">
         <f>SUM(G43:G47)</f>
         <v>15</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="L42" s="61"/>
-      <c r="M42" s="61" t="s">
-        <v>85</v>
-      </c>
-      <c r="N42" s="61"/>
+      <c r="K42" s="95" t="s">
+        <v>79</v>
+      </c>
+      <c r="L42" s="95"/>
+      <c r="M42" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="N42" s="95"/>
       <c r="O42" s="7"/>
       <c r="AMJ42"/>
     </row>
     <row r="43" spans="1:1024" s="4" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A43" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="63"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
+      <c r="A43" s="75" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="75"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="75"/>
       <c r="G43" s="18">
         <v>1</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I43" s="12" t="e">
         <f>A42+TIME(0,G43,0)</f>
@@ -5373,31 +5483,31 @@
         <f>J16</f>
         <v>{host_name}</v>
       </c>
-      <c r="K43" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="L43" s="61"/>
-      <c r="M43" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="N43" s="61"/>
+      <c r="K43" s="95" t="s">
+        <v>82</v>
+      </c>
+      <c r="L43" s="95"/>
+      <c r="M43" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="N43" s="95"/>
       <c r="O43" s="7"/>
       <c r="AMJ43"/>
     </row>
     <row r="44" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A44" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="B44" s="63"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
+      <c r="A44" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="75"/>
+      <c r="C44" s="75"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="75"/>
+      <c r="F44" s="75"/>
       <c r="G44" s="18">
         <v>2</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I44" s="12" t="e">
         <f>I43+TIME(0,G44,0)</f>
@@ -5407,30 +5517,30 @@
         <f>J17</f>
         <v>丘愉庄</v>
       </c>
-      <c r="K44" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="L44" s="61"/>
-      <c r="M44" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="N44" s="61"/>
+      <c r="K44" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="L44" s="95"/>
+      <c r="M44" s="95" t="s">
+        <v>86</v>
+      </c>
+      <c r="N44" s="95"/>
       <c r="AMJ44"/>
     </row>
     <row r="45" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A45" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
+      <c r="A45" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="75"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
       <c r="G45" s="18">
         <v>2</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I45" s="12" t="e">
         <f>I44+TIME(0,G45,0)</f>
@@ -5440,30 +5550,30 @@
         <f>J18</f>
         <v>xxx</v>
       </c>
-      <c r="K45" s="61" t="s">
-        <v>93</v>
-      </c>
-      <c r="L45" s="61"/>
-      <c r="M45" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="N45" s="61"/>
+      <c r="K45" s="95" t="s">
+        <v>88</v>
+      </c>
+      <c r="L45" s="95"/>
+      <c r="M45" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="N45" s="95"/>
       <c r="AMJ45"/>
     </row>
     <row r="46" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A46" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="B46" s="63"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
+      <c r="A46" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="75"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="75"/>
       <c r="G46" s="18">
         <v>3</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I46" s="12" t="e">
         <f>I45+TIME(0,G46,0)</f>
@@ -5473,69 +5583,69 @@
         <f>J19</f>
         <v>xxx</v>
       </c>
-      <c r="K46" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="L46" s="61"/>
-      <c r="M46" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="N46" s="61"/>
+      <c r="K46" s="95" t="s">
+        <v>91</v>
+      </c>
+      <c r="L46" s="95"/>
+      <c r="M46" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="N46" s="95"/>
       <c r="AMJ46"/>
     </row>
     <row r="47" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A47" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
+      <c r="A47" s="75" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="75"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
       <c r="G47" s="18">
         <v>7</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I47" s="12" t="e">
         <f>I46+TIME(0,G47,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K47" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="L47" s="61"/>
-      <c r="M47" s="65"/>
-      <c r="N47" s="65"/>
+        <v>47</v>
+      </c>
+      <c r="K47" s="95" t="s">
+        <v>94</v>
+      </c>
+      <c r="L47" s="95"/>
+      <c r="M47" s="96"/>
+      <c r="N47" s="96"/>
       <c r="AMJ47"/>
     </row>
     <row r="48" spans="1:1024" s="4" customFormat="1" ht="21.6" customHeight="1">
       <c r="A48" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="C48" s="66"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="66"/>
-      <c r="G48" s="66"/>
-      <c r="H48" s="66"/>
-      <c r="I48" s="66"/>
-      <c r="J48" s="66"/>
-      <c r="K48" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="L48" s="67"/>
-      <c r="M48" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="N48" s="67"/>
+        <v>95</v>
+      </c>
+      <c r="B48" s="97" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="97"/>
+      <c r="D48" s="97"/>
+      <c r="E48" s="97"/>
+      <c r="F48" s="97"/>
+      <c r="G48" s="97"/>
+      <c r="H48" s="97"/>
+      <c r="I48" s="97"/>
+      <c r="J48" s="97"/>
+      <c r="K48" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="L48" s="79"/>
+      <c r="M48" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="N48" s="79"/>
       <c r="AMJ48"/>
     </row>
     <row r="49" spans="1:1024" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -5543,127 +5653,127 @@
         <f>A42+TIME(0,G42,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B49" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60"/>
+      <c r="B49" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="80"/>
+      <c r="D49" s="80"/>
+      <c r="E49" s="80"/>
+      <c r="F49" s="80"/>
       <c r="G49" s="15">
         <f>SUM(G50:G52)</f>
         <v>8</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="17"/>
-      <c r="K49" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="L49" s="61"/>
-      <c r="M49" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="N49" s="61"/>
+      <c r="K49" s="95" t="s">
+        <v>100</v>
+      </c>
+      <c r="L49" s="95"/>
+      <c r="M49" s="95" t="s">
+        <v>101</v>
+      </c>
+      <c r="N49" s="95"/>
       <c r="AMJ49"/>
     </row>
     <row r="50" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A50" s="64" t="s">
-        <v>107</v>
-      </c>
-      <c r="B50" s="64"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
+      <c r="A50" s="89" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="89"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89"/>
       <c r="G50" s="28">
         <v>4</v>
       </c>
       <c r="H50" s="31" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I50" s="34" t="e">
         <f>A49+TIME(0,G50,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K50" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="L50" s="61"/>
-      <c r="M50" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="N50" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="K50" s="95" t="s">
+        <v>103</v>
+      </c>
+      <c r="L50" s="95"/>
+      <c r="M50" s="95" t="s">
+        <v>104</v>
+      </c>
+      <c r="N50" s="95"/>
       <c r="AMJ50"/>
     </row>
     <row r="51" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A51" s="62" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" s="62"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="62"/>
-      <c r="E51" s="62"/>
-      <c r="F51" s="62"/>
+      <c r="A51" s="100" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="100"/>
+      <c r="C51" s="100"/>
+      <c r="D51" s="100"/>
+      <c r="E51" s="100"/>
+      <c r="F51" s="100"/>
       <c r="G51" s="18">
         <v>3</v>
       </c>
       <c r="H51" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I51" s="12" t="e">
         <f>I50+TIME(0,G51,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K51" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="L51" s="61"/>
-      <c r="M51" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="N51" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="K51" s="95" t="s">
+        <v>106</v>
+      </c>
+      <c r="L51" s="95"/>
+      <c r="M51" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="N51" s="95"/>
       <c r="AMJ51"/>
     </row>
     <row r="52" spans="1:1024" s="4" customFormat="1" ht="19.350000000000001" customHeight="1">
-      <c r="A52" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
-      <c r="F52" s="63"/>
+      <c r="A52" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="75"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
       <c r="G52" s="18">
         <v>1</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I52" s="12" t="e">
         <f>I51+TIME(0,G52,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="K52" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="L52" s="61"/>
-      <c r="M52" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="N52" s="61"/>
-      <c r="O52" s="58"/>
+        <v>109</v>
+      </c>
+      <c r="K52" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="L52" s="95"/>
+      <c r="M52" s="95" t="s">
+        <v>111</v>
+      </c>
+      <c r="N52" s="95"/>
+      <c r="O52" s="98"/>
       <c r="AMJ52"/>
     </row>
     <row r="53" spans="1:1024" s="4" customFormat="1" ht="24" customHeight="1">
@@ -5671,30 +5781,30 @@
         <f>A49+TIME(0,G49,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B53" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
-      <c r="H53" s="60"/>
-      <c r="I53" s="60"/>
-      <c r="J53" s="60"/>
-      <c r="K53" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="L53" s="61"/>
-      <c r="M53" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="N53" s="61"/>
-      <c r="O53" s="58"/>
+      <c r="B53" s="80" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="80"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="80"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="80"/>
+      <c r="I53" s="80"/>
+      <c r="J53" s="80"/>
+      <c r="K53" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="L53" s="95"/>
+      <c r="M53" s="95" t="s">
+        <v>114</v>
+      </c>
+      <c r="N53" s="95"/>
+      <c r="O53" s="98"/>
       <c r="AMJ53"/>
     </row>
     <row r="54" spans="1:1024" ht="24" customHeight="1">
-      <c r="O54" s="59"/>
+      <c r="O54" s="99"/>
     </row>
     <row r="55" spans="1:1024" ht="24" customHeight="1"/>
     <row r="56" spans="1:1024" ht="24" customHeight="1"/>
@@ -5710,51 +5820,45 @@
     <row r="1048576" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="K9:N10"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="K25:N27"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="O52:O54"/>
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="B48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
     <mergeCell ref="A32:F32"/>
     <mergeCell ref="K32:N32"/>
     <mergeCell ref="A33:F33"/>
@@ -5766,51 +5870,57 @@
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A39:F39"/>
     <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="B48:J48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="M48:N48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="O52:O54"/>
-    <mergeCell ref="B53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="K25:N27"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="K9:N10"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="N1:N3"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0" right="6.9444444444444406E-2" top="0.6" bottom="0.65972222222222199" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" scale="60" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="63" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5818,8 +5928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5829,116 +5939,116 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>156</v>
+        <v>143</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>